<commit_message>
removed redaction of references to Wannon Water
</commit_message>
<xml_diff>
--- a/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
+++ b/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\advisory rfq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46F6212-8DF4-4E10-A28D-4751C52A426E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C860E211-9CEE-47C4-AA51-CC6C84F110F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51600" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{244677D2-74B4-4266-AB66-552EE3A0A616}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>EVALUATION CRITERIA</t>
   </si>
@@ -282,9 +282,6 @@
       </rPr>
       <t>Environmental</t>
     </r>
-  </si>
-  <si>
-    <t>TOTAL SCORE</t>
   </si>
   <si>
     <t>PART 2 - COMMERCIAL</t>
@@ -541,6 +538,13 @@
 That both parties agree to such an extension annually;
 That the period of extension is by mutual agreement.
 Wannon Water shall notify the Consultant in writing, a minimum of sixty (60) days prior to the end of the Contract period, of its wish to extend the Contract.  The Consultant shall notify Wannon Water in writing, within thirty (30) days of receiving the offer from Wannon Water, of its acceptance or otherwise of the offer to extend the Contract.</t>
+  </si>
+  <si>
+    <t>Higher score if company has previous worked with Wannon Water.</t>
+  </si>
+  <si>
+    <t>Higher score if company has previous worked with Wannon Water - this is important for continuity of delivery of Digital Operating Model and Digital Strategy.
+Lower score if company has not previous worked for Wannon Water.</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D7AF77-B56D-4660-ADBB-CDF91CBA8222}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,7 +1140,9 @@
         <v>5</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="289.8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1144,7 +1150,7 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="69" x14ac:dyDescent="0.25">
@@ -1153,7 +1159,7 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="69" x14ac:dyDescent="0.25">
@@ -1162,7 +1168,7 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1179,7 +1185,9 @@
         <v>10</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="17"/>
+      <c r="C10" s="17" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="317.39999999999998" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1187,7 +1195,7 @@
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="386.4" x14ac:dyDescent="0.25">
@@ -1196,7 +1204,7 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="138" x14ac:dyDescent="0.25">
@@ -1205,12 +1213,12 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="10">
         <v>20</v>
@@ -1223,7 +1231,7 @@
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -1232,7 +1240,7 @@
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1250,7 +1258,7 @@
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="96.6" x14ac:dyDescent="0.25">
@@ -1259,7 +1267,7 @@
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,57 +1286,57 @@
       <c r="A22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="13">
-        <v>100</v>
+      <c r="B22" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="C22" s="17"/>
     </row>
-    <row r="23" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="B23" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="C23" s="17"/>
     </row>
-    <row r="24" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="304.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="304.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="B26" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>22</v>
       </c>
       <c r="C27" s="17"/>
     </row>
@@ -1337,31 +1345,22 @@
         <v>28</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>26</v>
+      <c r="B29" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C26" r:id="rId1" display="https://content.vic.gov.au/sites/default/files/2023-12/eServcies-contract-%28April-2021%29.pdf" xr:uid="{870A90FF-5C17-47AB-8280-F8FC5CE1B5C0}"/>
+    <hyperlink ref="C25" r:id="rId1" display="https://content.vic.gov.au/sites/default/files/2023-12/eServcies-contract-%28April-2021%29.pdf" xr:uid="{870A90FF-5C17-47AB-8280-F8FC5CE1B5C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
removed redaction of references tothe company to allow for evaluction of previous working relationship but also redacted the contract number
</commit_message>
<xml_diff>
--- a/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
+++ b/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\advisory rfq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C860E211-9CEE-47C4-AA51-CC6C84F110F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A1B95-F917-43E3-A750-FF33A9F192E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51600" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{244677D2-74B4-4266-AB66-552EE3A0A616}"/>
   </bookViews>
@@ -543,7 +543,7 @@
     <t>Higher score if company has previous worked with Wannon Water.</t>
   </si>
   <si>
-    <t>Higher score if company has previous worked with Wannon Water - this is important for continuity of delivery of Digital Operating Model and Digital Strategy.
+    <t>Higher score if company has previous worked with Wannon Water - this is important for continuity of delivery of Digital Operating Model and Digital Strategy.  This may be shown in examples of previous partnering or partnerships. If evidence found then this criteria should be scored no lower than an 8.  If no evidence found then score this criteria no higher than a 7.
 Lower score if company has not previous worked for Wannon Water.</t>
   </si>
 </sst>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes to sub criteria for testing
</commit_message>
<xml_diff>
--- a/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
+++ b/documents/advisory rfq/AdvisoryEvalMatrix_incTenderBriefData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.dilley\development\evaluation\evaluation_2\documents\advisory rfq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A1B95-F917-43E3-A750-FF33A9F192E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD05F2CA-64E5-44E0-A1E3-80675F1D2AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51600" yWindow="3750" windowWidth="25800" windowHeight="21000" xr2:uid="{244677D2-74B4-4266-AB66-552EE3A0A616}"/>
   </bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc176179427" localSheetId="0">Sheet1!$C$15</definedName>
-    <definedName name="_Toc176179431" localSheetId="0">Sheet1!$C$12</definedName>
-    <definedName name="_Toc176179432" localSheetId="0">Sheet1!$C$16</definedName>
-    <definedName name="_Toc176179433" localSheetId="0">Sheet1!$C$19</definedName>
+    <definedName name="_Toc176179427" localSheetId="0">Sheet1!$C$16</definedName>
+    <definedName name="_Toc176179431" localSheetId="0">Sheet1!$C$13</definedName>
+    <definedName name="_Toc176179432" localSheetId="0">Sheet1!$C$17</definedName>
+    <definedName name="_Toc176179433" localSheetId="0">Sheet1!$C$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>EVALUATION CRITERIA</t>
   </si>
@@ -493,16 +493,6 @@
 Innovation and Updates: A demonstrated commitment to staying at the forefront of industry trends and updating services accordingly.</t>
   </si>
   <si>
-    <t xml:space="preserve">The service will be delivered through the following channels:
-Research Reports: Access to detailed reports on trends, best practices, and technologies in IT and OT.
-Market Analysis: Regular updates on the competitive landscape, including vendor evaluations, market forecasts, and technology adoption rates.
-Strategic Guidance: Customised strategic advice based on the latest industry trends and specific business needs.
-Benchmarking Services: Data and tools to compare Wannon Water's performance against industry peers.
-Access to Analysts: Direct consultations with industry experts for personalised advice and support.
-Workshops, Webinars, and Conferences: Access to world-class conferences, educational sessions, and workshops that provide cutting-edge insights and networking opportunities with industry leaders.
-</t>
-  </si>
-  <si>
     <t>An indication of how the service would be implemented.</t>
   </si>
   <si>
@@ -545,6 +535,22 @@
   <si>
     <t>Higher score if company has previous worked with Wannon Water - this is important for continuity of delivery of Digital Operating Model and Digital Strategy.  This may be shown in examples of previous partnering or partnerships. If evidence found then this criteria should be scored no lower than an 8.  If no evidence found then score this criteria no higher than a 7.
 Lower score if company has not previous worked for Wannon Water.</t>
+  </si>
+  <si>
+    <t>History of partnering with Wannon Water</t>
+  </si>
+  <si>
+    <t>Very important!</t>
+  </si>
+  <si>
+    <t>The service will be delivered through the following channels:
+Research Reports: Access to detailed reports on trends, best practices, and technologies in IT and OT.
+Market Analysis: Regular updates on the competitive landscape, including vendor evaluations, market forecasts, and technology adoption rates.
+Strategic Guidance: Customised strategic advice based on the latest industry trends and specific business needs.
+Benchmarking Services: Data and tools to compare Wannon Water's performance against industry peers.
+Access to Analysts: Direct consultations with industry experts for personalised advice and support.
+Workshops, Webinars, and Conferences: Access to world-class conferences, educational sessions, and workshops that provide cutting-edge insights and networking opportunities with industry leaders.
+Specifically call out the number of seats or employee access licences as part of the proposal.</t>
   </si>
 </sst>
 </file>
@@ -1088,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D7AF77-B56D-4660-ADBB-CDF91CBA8222}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1137,230 +1143,239 @@
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="289.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>6</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="289.8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B10" s="10">
         <v>35</v>
       </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="317.39999999999998" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="386.4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="331.2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="386.4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B15" s="10">
         <v>20</v>
       </c>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B18" s="10">
         <v>5</v>
       </c>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3" ht="138" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="138" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="96.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>18</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="11"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="17"/>
     </row>
     <row r="22" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="304.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="304.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B26" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="C26" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>25</v>
       </c>
       <c r="C27" s="17"/>
     </row>
     <row r="28" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B30" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C30" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C25" r:id="rId1" display="https://content.vic.gov.au/sites/default/files/2023-12/eServcies-contract-%28April-2021%29.pdf" xr:uid="{870A90FF-5C17-47AB-8280-F8FC5CE1B5C0}"/>
+    <hyperlink ref="C26" r:id="rId1" display="https://content.vic.gov.au/sites/default/files/2023-12/eServcies-contract-%28April-2021%29.pdf" xr:uid="{870A90FF-5C17-47AB-8280-F8FC5CE1B5C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>